<commit_message>
Added Signin Feature and Signout Feature
</commit_message>
<xml_diff>
--- a/src/test/java/com/ds/qa/testdata/registrationdata.xlsx
+++ b/src/test/java/com/ds/qa/testdata/registrationdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinth\eclipse-workspace\DS-Algo\src\test\java\com\ds\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E106EAA-115C-4A78-A356-5DCF17939B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4565DC-AF0B-4366-917F-33FFE8160E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E80D379D-01FE-4EFB-B833-0E49C0DF9C51}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{E80D379D-01FE-4EFB-B833-0E49C0DF9C51}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="signin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -93,6 +94,24 @@
   </si>
   <si>
     <t>cinthiya</t>
+  </si>
+  <si>
+    <t>cin@123</t>
+  </si>
+  <si>
+    <t>!@@#$</t>
+  </si>
+  <si>
+    <t>!@@#%</t>
+  </si>
+  <si>
+    <t>Dsportal@123</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>cinthiyaSDET85</t>
   </si>
 </sst>
 </file>
@@ -468,7 +487,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,10 +504,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -676,4 +695,115 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A39D309-862B-4224-A1B4-0FBE5B23871F}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{7FB21368-D9AE-4554-B6CC-2FF5E94D0AAA}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{9E3D631D-CB2F-4915-A70C-E05F6F45E45A}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{726E3AC0-F404-44AC-9F05-ACD0D3C260DC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>